<commit_message>
Further Optimizations and SST tracking
</commit_message>
<xml_diff>
--- a/Assets/SSTs.xlsx
+++ b/Assets/SSTs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="11520" windowHeight="10440"/>
+    <workbookView windowWidth="23040" windowHeight="9995"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="10" r:id="rId1"/>
@@ -27,12 +27,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
-  <si>
-    <t>SST Sheet - $01 (SonicPlayer)</t>
-  </si>
-  <si>
-    <t>SSTs used:</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="101">
+  <si>
+    <t>SST Sheet - $01 (Player)</t>
+  </si>
+  <si>
+    <t>Free SSTs</t>
   </si>
   <si>
     <t>00</t>
@@ -107,10 +107,10 @@
     <t>obVelX</t>
   </si>
   <si>
-    <t>obVely</t>
-  </si>
-  <si>
-    <t>obRespawnNo</t>
+    <t>obVelY</t>
+  </si>
+  <si>
+    <t>obRespawnAddr</t>
   </si>
   <si>
     <t>obHeight</t>
@@ -155,13 +155,181 @@
     <t>obRoutine</t>
   </si>
   <si>
-    <t>ob2ndRout</t>
+    <t>DblJumpProp</t>
   </si>
   <si>
     <t>obAngle</t>
   </si>
   <si>
+    <t>SpinDashCtr</t>
+  </si>
+  <si>
+    <t>DblJumpFlag</t>
+  </si>
+  <si>
     <t>30</t>
+  </si>
+  <si>
+    <t>obInvuln</t>
+  </si>
+  <si>
+    <t>obInvinc</t>
+  </si>
+  <si>
+    <t>obShoes</t>
+  </si>
+  <si>
+    <t>obfrontAngle</t>
+  </si>
+  <si>
+    <t>obRearAngle</t>
+  </si>
+  <si>
+    <t>obOnWheel</t>
+  </si>
+  <si>
+    <t>obStatus2nd</t>
+  </si>
+  <si>
+    <t>obRestartTimer</t>
+  </si>
+  <si>
+    <t>obJumping</t>
+  </si>
+  <si>
+    <t>obLRLock</t>
+  </si>
+  <si>
+    <t>obPlatformAddr</t>
+  </si>
+  <si>
+    <t>SST Sheet - $03 (Path Swapper)</t>
+  </si>
+  <si>
+    <t>We might assume that other bytes after $34 may be used after $34(a0) is loaded to a2.</t>
+  </si>
+  <si>
+    <t>obSubtype</t>
+  </si>
+  <si>
+    <t>objoff_32</t>
+  </si>
+  <si>
+    <t>objoff_34</t>
+  </si>
+  <si>
+    <t>SST Sheet - $07 (Dust Effects)</t>
+  </si>
+  <si>
+    <t>$3C/3D are unused, but would be needed if a second player is added to the game.</t>
+  </si>
+  <si>
+    <t>objoff_3C</t>
+  </si>
+  <si>
+    <t>SST Sheet - $08 (Water Surface)</t>
+  </si>
+  <si>
+    <t>SST Sheet - $09 (Sp. Stage Player)</t>
+  </si>
+  <si>
+    <t>objoff_30</t>
+  </si>
+  <si>
+    <t>objoff_36</t>
+  </si>
+  <si>
+    <t>objoff_37</t>
+  </si>
+  <si>
+    <t>objoff_38</t>
+  </si>
+  <si>
+    <t>objoff_3A</t>
+  </si>
+  <si>
+    <t>SST Sheet - $0A (Drown Count)</t>
+  </si>
+  <si>
+    <t>objoff_2C</t>
+  </si>
+  <si>
+    <t>drown_origX</t>
+  </si>
+  <si>
+    <t>objoff_33</t>
+  </si>
+  <si>
+    <t>drown_time</t>
+  </si>
+  <si>
+    <t>SST Sheet - $0B (LZ Break Pole)</t>
+  </si>
+  <si>
+    <t>obColType</t>
+  </si>
+  <si>
+    <t>obColProp</t>
+  </si>
+  <si>
+    <t>pole_time</t>
+  </si>
+  <si>
+    <t>pole_grabbed</t>
+  </si>
+  <si>
+    <t>SST Sheet - $0C (LZ Flapping Door)</t>
+  </si>
+  <si>
+    <t>flap_wait</t>
+  </si>
+  <si>
+    <t>flap_time</t>
+  </si>
+  <si>
+    <t>SST Sheet - $0D (Signpost)</t>
+  </si>
+  <si>
+    <t>spintime</t>
+  </si>
+  <si>
+    <t>sparkletime</t>
+  </si>
+  <si>
+    <t>sparkle_id</t>
+  </si>
+  <si>
+    <t>SST Sheet - $0E (Title Sonic)</t>
+  </si>
+  <si>
+    <t>SST Sheet - $0F (PRESS START)</t>
+  </si>
+  <si>
+    <t>SST Sheet - $11 (GHZ Bridge)</t>
+  </si>
+  <si>
+    <t>Uses Subsprites (Check SST of subsprite instances)</t>
+  </si>
+  <si>
+    <t>obBriChild1</t>
+  </si>
+  <si>
+    <t>obBriChild2</t>
+  </si>
+  <si>
+    <t>objoff_3E</t>
+  </si>
+  <si>
+    <t>objoff_3F</t>
+  </si>
+  <si>
+    <t>SST Sheet - $12 (SYZ Light)</t>
+  </si>
+  <si>
+    <t>SST Sheet - $13 (MZ Ball Maker)</t>
+  </si>
+  <si>
+    <t>SST Sheet - $14 (MZ Lava Ball)</t>
   </si>
 </sst>
 </file>
@@ -174,7 +342,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -191,6 +359,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="8"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -342,7 +518,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -352,6 +528,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="0.05"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -542,7 +748,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -608,19 +814,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color auto="1"/>
       </left>
@@ -647,12 +840,14 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right/>
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -697,9 +892,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
+      <left/>
       <right style="medium">
         <color auto="1"/>
       </right>
@@ -827,73 +1020,58 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -902,62 +1080,77 @@
     <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -968,36 +1161,67 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1353,15 +1577,17 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:R6"/>
+  <dimension ref="A1:R104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="H79" sqref="H79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="5"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="1.77777777777778" customWidth="1"/>
+    <col min="2" max="2" width="4.88888888888889" customWidth="1"/>
+    <col min="3" max="18" width="11.2777777777778" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.15" spans="1:7">
@@ -1374,8 +1600,9 @@
       <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="2">
-        <v>0</v>
+      <c r="F1" s="2" t="str">
+        <f>DEC2HEX(COUNTBLANK(C3:R6))</f>
+        <v>A</v>
       </c>
       <c r="G1" s="2" t="str">
         <f>DEC2HEX(64)</f>
@@ -1411,25 +1638,25 @@
       <c r="K2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="12" t="s">
+      <c r="L2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="13" t="s">
+      <c r="M2" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="14" t="s">
+      <c r="N2" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="14" t="s">
+      <c r="O2" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="14" t="s">
+      <c r="P2" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="14" t="s">
+      <c r="Q2" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="R2" s="16" t="s">
+      <c r="R2" s="22" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1440,74 +1667,102 @@
       <c r="C3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="P3" s="15"/>
-      <c r="Q3" s="15"/>
-      <c r="R3" s="17"/>
+      <c r="F3" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="N3" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="O3" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="P3" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="R3" s="23" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="4" spans="2:18">
       <c r="B4" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="8" t="s">
+      <c r="D4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="9"/>
+      <c r="F4" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="G4" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="9"/>
-      <c r="I4" s="7" t="s">
+      <c r="H4" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="J4" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="K4" s="8" t="s">
+      <c r="K4" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="L4" s="9"/>
-      <c r="M4" s="7" t="s">
+      <c r="L4" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="M4" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="N4" s="7" t="s">
+      <c r="N4" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="O4" s="7" t="s">
+      <c r="O4" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="P4" s="7" t="s">
+      <c r="P4" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="Q4" s="7" t="s">
+      <c r="Q4" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="R4" s="18" t="s">
+      <c r="R4" s="24" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1515,68 +1770,3136 @@
       <c r="B5" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="7" t="s">
+      <c r="D5" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="I5" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="18"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="N5" s="13"/>
+      <c r="O5" s="13"/>
+      <c r="P5" s="13"/>
+      <c r="Q5" s="13"/>
+      <c r="R5" s="25" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="6" ht="15.15" spans="2:18">
       <c r="B6" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="11"/>
-      <c r="O6" s="11"/>
-      <c r="P6" s="11"/>
-      <c r="Q6" s="11"/>
-      <c r="R6" s="19"/>
+        <v>46</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="L6" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="M6" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="N6" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="O6" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="P6" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q6" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="R6" s="11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" ht="15.15" spans="1:8">
+      <c r="A8" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" s="2" t="str">
+        <f>DEC2HEX(COUNTBLANK(C10:R13))</f>
+        <v>25</v>
+      </c>
+      <c r="G8" s="2" t="str">
+        <f>DEC2HEX(64)</f>
+        <v>40</v>
+      </c>
+      <c r="H8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18">
+      <c r="B9" s="3"/>
+      <c r="C9" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M9" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="N9" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="O9" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="P9" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q9" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="R9" s="22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18">
+      <c r="B10" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K10" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="L10" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="M10" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="N10" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="O10" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="P10" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q10" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="R10" s="23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18">
+      <c r="B11" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="L11" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="M11" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="N11" s="13"/>
+      <c r="O11" s="13"/>
+      <c r="P11" s="13"/>
+      <c r="Q11" s="13"/>
+      <c r="R11" s="26"/>
+    </row>
+    <row r="12" spans="2:18">
+      <c r="B12" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="13"/>
+      <c r="P12" s="13"/>
+      <c r="Q12" s="13"/>
+      <c r="R12" s="26"/>
+    </row>
+    <row r="13" ht="15.15" spans="2:18">
+      <c r="B13" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12"/>
+      <c r="N13" s="12"/>
+      <c r="O13" s="12"/>
+      <c r="P13" s="12"/>
+      <c r="Q13" s="12"/>
+      <c r="R13" s="27"/>
+    </row>
+    <row r="15" ht="15.15" spans="1:8">
+      <c r="A15" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" t="s">
+        <v>1</v>
+      </c>
+      <c r="F15" s="2" t="str">
+        <f>DEC2HEX(COUNTBLANK(C17:R20))</f>
+        <v>1F</v>
+      </c>
+      <c r="G15" s="2" t="str">
+        <f>DEC2HEX(64)</f>
+        <v>40</v>
+      </c>
+      <c r="H15" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18">
+      <c r="B16" s="3"/>
+      <c r="C16" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L16" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M16" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="N16" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="O16" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="P16" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q16" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="R16" s="22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="2:18">
+      <c r="B17" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K17" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="L17" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="M17" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="N17" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="O17" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="P17" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q17" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="R17" s="23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="2:18">
+      <c r="B18" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="L18" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="M18" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="N18" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="O18" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="P18" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q18" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="R18" s="24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="2:18">
+      <c r="B19" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="L19" s="13"/>
+      <c r="M19" s="13"/>
+      <c r="N19" s="13"/>
+      <c r="O19" s="13"/>
+      <c r="P19" s="13"/>
+      <c r="Q19" s="13"/>
+      <c r="R19" s="26"/>
+    </row>
+    <row r="20" ht="15.15" spans="2:18">
+      <c r="B20" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="12"/>
+      <c r="N20" s="12"/>
+      <c r="O20" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="P20" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q20" s="12"/>
+      <c r="R20" s="27"/>
+    </row>
+    <row r="22" ht="15.15" spans="1:7">
+      <c r="A22" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" t="s">
+        <v>1</v>
+      </c>
+      <c r="F22" s="2" t="str">
+        <f>DEC2HEX(COUNTBLANK(C24:R27))</f>
+        <v>24</v>
+      </c>
+      <c r="G22" s="2" t="str">
+        <f>DEC2HEX(64)</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="2:18">
+      <c r="B23" s="3"/>
+      <c r="C23" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K23" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L23" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M23" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="N23" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="O23" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="P23" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q23" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="R23" s="22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="2:18">
+      <c r="B24" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="J24" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K24" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="L24" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="M24" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="N24" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="O24" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="P24" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q24" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="R24" s="23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="2:18">
+      <c r="B25" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H25" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I25" s="13"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="L25" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="M25" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="N25" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="O25" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="P25" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q25" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="R25" s="24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="2:18">
+      <c r="B26" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G26" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H26" s="13"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="13"/>
+      <c r="K26" s="13"/>
+      <c r="L26" s="13"/>
+      <c r="M26" s="13"/>
+      <c r="N26" s="13"/>
+      <c r="O26" s="13"/>
+      <c r="P26" s="13"/>
+      <c r="Q26" s="13"/>
+      <c r="R26" s="26"/>
+    </row>
+    <row r="27" ht="15.15" spans="2:18">
+      <c r="B27" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="12"/>
+      <c r="L27" s="12"/>
+      <c r="M27" s="12"/>
+      <c r="N27" s="12"/>
+      <c r="O27" s="12"/>
+      <c r="P27" s="12"/>
+      <c r="Q27" s="12"/>
+      <c r="R27" s="27"/>
+    </row>
+    <row r="29" ht="15.15" spans="1:7">
+      <c r="A29" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F29" s="2" t="str">
+        <f>DEC2HEX(COUNTBLANK(C31:R34))</f>
+        <v>17</v>
+      </c>
+      <c r="G29" s="2" t="str">
+        <f>DEC2HEX(64)</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="2:18">
+      <c r="B30" s="3"/>
+      <c r="C30" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J30" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K30" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L30" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M30" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="N30" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="O30" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="P30" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q30" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="R30" s="22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="2:18">
+      <c r="B31" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I31" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="J31" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K31" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="L31" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="M31" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="N31" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="O31" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="P31" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q31" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="R31" s="23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="2:18">
+      <c r="B32" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H32" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I32" s="13"/>
+      <c r="J32" s="13"/>
+      <c r="K32" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="L32" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="M32" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="N32" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="O32" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="P32" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q32" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="R32" s="24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="2:18">
+      <c r="B33" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G33" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H33" s="13"/>
+      <c r="I33" s="13"/>
+      <c r="J33" s="13"/>
+      <c r="K33" s="13"/>
+      <c r="L33" s="13"/>
+      <c r="M33" s="13"/>
+      <c r="N33" s="13"/>
+      <c r="O33" s="13"/>
+      <c r="P33" s="13"/>
+      <c r="Q33" s="13"/>
+      <c r="R33" s="26"/>
+    </row>
+    <row r="34" ht="15.15" spans="2:18">
+      <c r="B34" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="D34" s="12"/>
+      <c r="E34" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="F34" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="G34" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="H34" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="I34" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="J34" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="K34" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="L34" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="M34" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="N34" s="12"/>
+      <c r="O34" s="12"/>
+      <c r="P34" s="12"/>
+      <c r="Q34" s="12"/>
+      <c r="R34" s="27"/>
+    </row>
+    <row r="36" ht="15.15" spans="1:7">
+      <c r="A36" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" t="s">
+        <v>1</v>
+      </c>
+      <c r="F36" s="2" t="str">
+        <f>DEC2HEX(COUNTBLANK(C38:R41))</f>
+        <v>15</v>
+      </c>
+      <c r="G36" s="2" t="str">
+        <f>DEC2HEX(64)</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="2:18">
+      <c r="B37" s="3"/>
+      <c r="C37" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I37" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J37" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K37" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L37" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M37" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="N37" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="O37" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="P37" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q37" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="R37" s="22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="38" spans="2:18">
+      <c r="B38" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G38" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H38" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I38" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="J38" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K38" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="L38" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="M38" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="N38" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="O38" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="P38" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q38" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="R38" s="23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="2:18">
+      <c r="B39" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C39" s="13"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="13"/>
+      <c r="F39" s="13"/>
+      <c r="G39" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H39" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I39" s="13"/>
+      <c r="J39" s="13"/>
+      <c r="K39" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="L39" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="M39" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="N39" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="O39" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="P39" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q39" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="R39" s="24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="40" spans="2:18">
+      <c r="B40" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C40" s="13"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G40" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H40" s="13"/>
+      <c r="I40" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="J40" s="13"/>
+      <c r="K40" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="L40" s="13"/>
+      <c r="M40" s="13"/>
+      <c r="N40" s="13"/>
+      <c r="O40" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="P40" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q40" s="13"/>
+      <c r="R40" s="26"/>
+    </row>
+    <row r="41" ht="15.15" spans="2:18">
+      <c r="B41" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C41" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="D41" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="E41" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="F41" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="G41" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="H41" s="12"/>
+      <c r="I41" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="J41" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="K41" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="L41" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="M41" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="N41" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="O41" s="12"/>
+      <c r="P41" s="12"/>
+      <c r="Q41" s="12"/>
+      <c r="R41" s="27"/>
+    </row>
+    <row r="43" ht="15.15" spans="1:7">
+      <c r="A43" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" t="s">
+        <v>1</v>
+      </c>
+      <c r="F43" s="2" t="str">
+        <f>DEC2HEX(COUNTBLANK(C45:R48))</f>
+        <v>23</v>
+      </c>
+      <c r="G43" s="2" t="str">
+        <f>DEC2HEX(64)</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="44" spans="2:18">
+      <c r="B44" s="3"/>
+      <c r="C44" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G44" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H44" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I44" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J44" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K44" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L44" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M44" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="N44" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="O44" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="P44" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q44" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="R44" s="22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="45" spans="2:18">
+      <c r="B45" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F45" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G45" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H45" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I45" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="J45" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K45" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="L45" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="M45" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="N45" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="O45" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="P45" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q45" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="R45" s="23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="46" spans="2:18">
+      <c r="B46" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C46" s="13"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H46" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I46" s="13"/>
+      <c r="J46" s="13"/>
+      <c r="K46" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="L46" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="M46" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="N46" s="13"/>
+      <c r="O46" s="13"/>
+      <c r="P46" s="13"/>
+      <c r="Q46" s="13"/>
+      <c r="R46" s="26"/>
+    </row>
+    <row r="47" spans="2:18">
+      <c r="B47" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C47" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="D47" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="E47" s="13"/>
+      <c r="F47" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G47" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H47" s="13"/>
+      <c r="I47" s="13"/>
+      <c r="J47" s="13"/>
+      <c r="K47" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="L47" s="13"/>
+      <c r="M47" s="13"/>
+      <c r="N47" s="13"/>
+      <c r="O47" s="13"/>
+      <c r="P47" s="13"/>
+      <c r="Q47" s="13"/>
+      <c r="R47" s="26"/>
+    </row>
+    <row r="48" ht="15.15" spans="2:18">
+      <c r="B48" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C48" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="D48" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="E48" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="F48" s="12"/>
+      <c r="G48" s="12"/>
+      <c r="H48" s="12"/>
+      <c r="I48" s="12"/>
+      <c r="J48" s="12"/>
+      <c r="K48" s="12"/>
+      <c r="L48" s="12"/>
+      <c r="M48" s="12"/>
+      <c r="N48" s="12"/>
+      <c r="O48" s="12"/>
+      <c r="P48" s="12"/>
+      <c r="Q48" s="12"/>
+      <c r="R48" s="27"/>
+    </row>
+    <row r="50" ht="15.15" spans="1:7">
+      <c r="A50" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" t="s">
+        <v>1</v>
+      </c>
+      <c r="F50" s="2" t="str">
+        <f>DEC2HEX(COUNTBLANK(C52:R55))</f>
+        <v>1F</v>
+      </c>
+      <c r="G50" s="2" t="str">
+        <f>DEC2HEX(64)</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="51" spans="2:18">
+      <c r="B51" s="3"/>
+      <c r="C51" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G51" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H51" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I51" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J51" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K51" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L51" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M51" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="N51" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="O51" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="P51" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q51" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="R51" s="22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="52" spans="2:18">
+      <c r="B52" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F52" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G52" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H52" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I52" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="J52" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K52" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="L52" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="M52" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="N52" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="O52" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="P52" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q52" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="R52" s="23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="53" spans="2:18">
+      <c r="B53" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C53" s="13"/>
+      <c r="D53" s="13"/>
+      <c r="E53" s="13"/>
+      <c r="F53" s="13"/>
+      <c r="G53" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H53" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I53" s="13"/>
+      <c r="J53" s="13"/>
+      <c r="K53" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="L53" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="M53" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="N53" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="O53" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="P53" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q53" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="R53" s="24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="54" spans="2:18">
+      <c r="B54" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C54" s="13"/>
+      <c r="D54" s="13"/>
+      <c r="E54" s="13"/>
+      <c r="F54" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G54" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H54" s="13"/>
+      <c r="I54" s="13"/>
+      <c r="J54" s="13"/>
+      <c r="K54" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="L54" s="13"/>
+      <c r="M54" s="13"/>
+      <c r="N54" s="13"/>
+      <c r="O54" s="13"/>
+      <c r="P54" s="13"/>
+      <c r="Q54" s="13"/>
+      <c r="R54" s="26"/>
+    </row>
+    <row r="55" ht="15.15" spans="2:18">
+      <c r="B55" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C55" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="D55" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="E55" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="F55" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="G55" s="12"/>
+      <c r="H55" s="12"/>
+      <c r="I55" s="12"/>
+      <c r="J55" s="12"/>
+      <c r="K55" s="12"/>
+      <c r="L55" s="12"/>
+      <c r="M55" s="12"/>
+      <c r="N55" s="12"/>
+      <c r="O55" s="12"/>
+      <c r="P55" s="12"/>
+      <c r="Q55" s="12"/>
+      <c r="R55" s="27"/>
+    </row>
+    <row r="57" ht="15.15" spans="1:7">
+      <c r="A57" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" t="s">
+        <v>1</v>
+      </c>
+      <c r="F57" s="2" t="str">
+        <f>DEC2HEX(COUNTBLANK(C59:R62))</f>
+        <v>1F</v>
+      </c>
+      <c r="G57" s="2" t="str">
+        <f>DEC2HEX(64)</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="58" spans="2:18">
+      <c r="B58" s="3"/>
+      <c r="C58" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F58" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G58" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H58" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I58" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J58" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K58" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L58" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M58" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="N58" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="O58" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="P58" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q58" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="R58" s="22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="59" spans="2:18">
+      <c r="B59" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E59" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F59" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G59" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H59" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I59" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="J59" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K59" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="L59" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="M59" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="N59" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="O59" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="P59" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q59" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="R59" s="23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="60" spans="2:18">
+      <c r="B60" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C60" s="13"/>
+      <c r="D60" s="13"/>
+      <c r="E60" s="13"/>
+      <c r="F60" s="13"/>
+      <c r="G60" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H60" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I60" s="13"/>
+      <c r="J60" s="13"/>
+      <c r="K60" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="L60" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="M60" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="N60" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="O60" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="P60" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q60" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="R60" s="24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="61" spans="2:18">
+      <c r="B61" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C61" s="13"/>
+      <c r="D61" s="13"/>
+      <c r="E61" s="13"/>
+      <c r="F61" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G61" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H61" s="13"/>
+      <c r="I61" s="13"/>
+      <c r="J61" s="13"/>
+      <c r="K61" s="13"/>
+      <c r="L61" s="13"/>
+      <c r="M61" s="13"/>
+      <c r="N61" s="13"/>
+      <c r="O61" s="13"/>
+      <c r="P61" s="13"/>
+      <c r="Q61" s="13"/>
+      <c r="R61" s="26"/>
+    </row>
+    <row r="62" ht="15.15" spans="2:18">
+      <c r="B62" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C62" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="D62" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="E62" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="F62" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="G62" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="H62" s="12"/>
+      <c r="I62" s="12"/>
+      <c r="J62" s="12"/>
+      <c r="K62" s="12"/>
+      <c r="L62" s="12"/>
+      <c r="M62" s="12"/>
+      <c r="N62" s="12"/>
+      <c r="O62" s="12"/>
+      <c r="P62" s="12"/>
+      <c r="Q62" s="12"/>
+      <c r="R62" s="27"/>
+    </row>
+    <row r="64" ht="15.15" spans="1:7">
+      <c r="A64" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B64" s="1"/>
+      <c r="C64" s="1"/>
+      <c r="D64" s="1"/>
+      <c r="E64" t="s">
+        <v>1</v>
+      </c>
+      <c r="F64" s="2" t="str">
+        <f>DEC2HEX(COUNTBLANK(C66:R69))</f>
+        <v>24</v>
+      </c>
+      <c r="G64" s="2" t="str">
+        <f>DEC2HEX(64)</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="65" spans="2:18">
+      <c r="B65" s="3"/>
+      <c r="C65" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E65" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F65" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G65" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H65" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I65" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J65" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K65" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L65" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M65" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="N65" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="O65" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="P65" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q65" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="R65" s="22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="66" spans="2:18">
+      <c r="B66" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D66" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E66" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F66" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G66" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H66" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I66" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="J66" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K66" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="L66" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="M66" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="N66" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="O66" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="P66" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q66" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="R66" s="23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="67" spans="2:18">
+      <c r="B67" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C67" s="13"/>
+      <c r="D67" s="13"/>
+      <c r="E67" s="13"/>
+      <c r="F67" s="13"/>
+      <c r="G67" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H67" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I67" s="13"/>
+      <c r="J67" s="13"/>
+      <c r="K67" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="L67" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="M67" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="N67" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="O67" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="P67" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q67" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="R67" s="24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="68" spans="2:18">
+      <c r="B68" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C68" s="13"/>
+      <c r="D68" s="13"/>
+      <c r="E68" s="13"/>
+      <c r="F68" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G68" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H68" s="13"/>
+      <c r="I68" s="13"/>
+      <c r="J68" s="13"/>
+      <c r="K68" s="13"/>
+      <c r="L68" s="13"/>
+      <c r="M68" s="13"/>
+      <c r="N68" s="13"/>
+      <c r="O68" s="13"/>
+      <c r="P68" s="13"/>
+      <c r="Q68" s="13"/>
+      <c r="R68" s="26"/>
+    </row>
+    <row r="69" ht="15.15" spans="2:18">
+      <c r="B69" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C69" s="12"/>
+      <c r="D69" s="12"/>
+      <c r="E69" s="12"/>
+      <c r="F69" s="12"/>
+      <c r="G69" s="12"/>
+      <c r="H69" s="12"/>
+      <c r="I69" s="12"/>
+      <c r="J69" s="12"/>
+      <c r="K69" s="12"/>
+      <c r="L69" s="12"/>
+      <c r="M69" s="12"/>
+      <c r="N69" s="12"/>
+      <c r="O69" s="12"/>
+      <c r="P69" s="12"/>
+      <c r="Q69" s="12"/>
+      <c r="R69" s="27"/>
+    </row>
+    <row r="71" ht="15.15" spans="1:7">
+      <c r="A71" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B71" s="1"/>
+      <c r="C71" s="1"/>
+      <c r="D71" s="1"/>
+      <c r="E71" t="s">
+        <v>1</v>
+      </c>
+      <c r="F71" s="2" t="str">
+        <f>DEC2HEX(COUNTBLANK(C73:R76))</f>
+        <v>24</v>
+      </c>
+      <c r="G71" s="2" t="str">
+        <f>DEC2HEX(64)</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="72" spans="2:18">
+      <c r="B72" s="3"/>
+      <c r="C72" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E72" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F72" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G72" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H72" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I72" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J72" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K72" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L72" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M72" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="N72" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="O72" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="P72" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q72" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="R72" s="22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="73" spans="2:18">
+      <c r="B73" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C73" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D73" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E73" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F73" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G73" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H73" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I73" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="J73" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K73" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="L73" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="M73" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="N73" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="O73" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="P73" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q73" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="R73" s="23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="74" spans="2:18">
+      <c r="B74" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C74" s="13"/>
+      <c r="D74" s="13"/>
+      <c r="E74" s="13"/>
+      <c r="F74" s="13"/>
+      <c r="G74" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H74" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I74" s="13"/>
+      <c r="J74" s="13"/>
+      <c r="K74" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="L74" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="M74" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="N74" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="O74" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="P74" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q74" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="R74" s="24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="75" spans="2:18">
+      <c r="B75" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C75" s="13"/>
+      <c r="D75" s="13"/>
+      <c r="E75" s="13"/>
+      <c r="F75" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G75" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H75" s="13"/>
+      <c r="I75" s="13"/>
+      <c r="J75" s="13"/>
+      <c r="K75" s="13"/>
+      <c r="L75" s="13"/>
+      <c r="M75" s="13"/>
+      <c r="N75" s="13"/>
+      <c r="O75" s="13"/>
+      <c r="P75" s="13"/>
+      <c r="Q75" s="13"/>
+      <c r="R75" s="26"/>
+    </row>
+    <row r="76" ht="15.15" spans="2:18">
+      <c r="B76" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C76" s="12"/>
+      <c r="D76" s="12"/>
+      <c r="E76" s="12"/>
+      <c r="F76" s="12"/>
+      <c r="G76" s="12"/>
+      <c r="H76" s="12"/>
+      <c r="I76" s="12"/>
+      <c r="J76" s="12"/>
+      <c r="K76" s="12"/>
+      <c r="L76" s="12"/>
+      <c r="M76" s="12"/>
+      <c r="N76" s="12"/>
+      <c r="O76" s="12"/>
+      <c r="P76" s="12"/>
+      <c r="Q76" s="12"/>
+      <c r="R76" s="27"/>
+    </row>
+    <row r="78" ht="15.15" spans="1:8">
+      <c r="A78" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B78" s="1"/>
+      <c r="C78" s="1"/>
+      <c r="D78" s="1"/>
+      <c r="E78" t="s">
+        <v>1</v>
+      </c>
+      <c r="F78" s="2" t="str">
+        <f>DEC2HEX(COUNTBLANK(C80:R83))</f>
+        <v>1B</v>
+      </c>
+      <c r="G78" s="2" t="str">
+        <f>DEC2HEX(64)</f>
+        <v>40</v>
+      </c>
+      <c r="H78" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="79" spans="2:18">
+      <c r="B79" s="3"/>
+      <c r="C79" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D79" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E79" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F79" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G79" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H79" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I79" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J79" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K79" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L79" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M79" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="N79" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="O79" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="P79" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q79" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="R79" s="22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="80" spans="2:18">
+      <c r="B80" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C80" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D80" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E80" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F80" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G80" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H80" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I80" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="J80" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K80" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="L80" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="M80" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="N80" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="O80" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="P80" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q80" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="R80" s="23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="81" spans="2:18">
+      <c r="B81" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C81" s="13"/>
+      <c r="D81" s="13"/>
+      <c r="E81" s="13"/>
+      <c r="F81" s="13"/>
+      <c r="G81" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H81" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I81" s="13"/>
+      <c r="J81" s="13"/>
+      <c r="K81" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="L81" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="M81" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="N81" s="13"/>
+      <c r="O81" s="13"/>
+      <c r="P81" s="13"/>
+      <c r="Q81" s="13"/>
+      <c r="R81" s="26"/>
+    </row>
+    <row r="82" spans="2:18">
+      <c r="B82" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C82" s="13"/>
+      <c r="D82" s="13"/>
+      <c r="E82" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F82" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G82" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H82" s="13"/>
+      <c r="I82" s="13"/>
+      <c r="J82" s="13"/>
+      <c r="K82" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="L82" s="13"/>
+      <c r="M82" s="13"/>
+      <c r="N82" s="13"/>
+      <c r="O82" s="13"/>
+      <c r="P82" s="13"/>
+      <c r="Q82" s="13"/>
+      <c r="R82" s="26"/>
+    </row>
+    <row r="83" ht="15.15" spans="2:18">
+      <c r="B83" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C83" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="D83" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="E83" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="F83" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="G83" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="H83" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="I83" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="J83" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="K83" s="12"/>
+      <c r="L83" s="12"/>
+      <c r="M83" s="12"/>
+      <c r="N83" s="12"/>
+      <c r="O83" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="P83" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q83" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="R83" s="28" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="85" ht="15.15" spans="1:7">
+      <c r="A85" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B85" s="1"/>
+      <c r="C85" s="1"/>
+      <c r="D85" s="1"/>
+      <c r="E85" t="s">
+        <v>1</v>
+      </c>
+      <c r="F85" s="2" t="str">
+        <f>DEC2HEX(COUNTBLANK(C87:R90))</f>
+        <v>28</v>
+      </c>
+      <c r="G85" s="2" t="str">
+        <f>DEC2HEX(64)</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="86" spans="2:18">
+      <c r="B86" s="3"/>
+      <c r="C86" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D86" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E86" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F86" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G86" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H86" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I86" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J86" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K86" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L86" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M86" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="N86" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="O86" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="P86" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q86" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="R86" s="22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="87" spans="2:18">
+      <c r="B87" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C87" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D87" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E87" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F87" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G87" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H87" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I87" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="J87" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K87" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="L87" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="M87" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="N87" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="O87" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="P87" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q87" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="R87" s="23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="88" spans="2:18">
+      <c r="B88" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C88" s="13"/>
+      <c r="D88" s="13"/>
+      <c r="E88" s="13"/>
+      <c r="F88" s="13"/>
+      <c r="G88" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H88" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I88" s="13"/>
+      <c r="J88" s="13"/>
+      <c r="K88" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="L88" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="M88" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="N88" s="13"/>
+      <c r="O88" s="13"/>
+      <c r="P88" s="13"/>
+      <c r="Q88" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="R88" s="26"/>
+    </row>
+    <row r="89" spans="2:18">
+      <c r="B89" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C89" s="13"/>
+      <c r="D89" s="13"/>
+      <c r="E89" s="13"/>
+      <c r="F89" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G89" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H89" s="13"/>
+      <c r="I89" s="13"/>
+      <c r="J89" s="13"/>
+      <c r="K89" s="13"/>
+      <c r="L89" s="13"/>
+      <c r="M89" s="13"/>
+      <c r="N89" s="13"/>
+      <c r="O89" s="13"/>
+      <c r="P89" s="13"/>
+      <c r="Q89" s="13"/>
+      <c r="R89" s="26"/>
+    </row>
+    <row r="90" ht="15.15" spans="2:18">
+      <c r="B90" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C90" s="12"/>
+      <c r="D90" s="12"/>
+      <c r="E90" s="12"/>
+      <c r="F90" s="12"/>
+      <c r="G90" s="12"/>
+      <c r="H90" s="12"/>
+      <c r="I90" s="12"/>
+      <c r="J90" s="12"/>
+      <c r="K90" s="12"/>
+      <c r="L90" s="12"/>
+      <c r="M90" s="12"/>
+      <c r="N90" s="12"/>
+      <c r="O90" s="12"/>
+      <c r="P90" s="12"/>
+      <c r="Q90" s="12"/>
+      <c r="R90" s="27"/>
+    </row>
+    <row r="92" ht="15.15" spans="1:7">
+      <c r="A92" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B92" s="1"/>
+      <c r="C92" s="1"/>
+      <c r="D92" s="1"/>
+      <c r="E92" t="s">
+        <v>1</v>
+      </c>
+      <c r="F92" s="2" t="str">
+        <f>DEC2HEX(COUNTBLANK(C94:R97))</f>
+        <v>26</v>
+      </c>
+      <c r="G92" s="2" t="str">
+        <f>DEC2HEX(64)</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="93" spans="2:18">
+      <c r="B93" s="3"/>
+      <c r="C93" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D93" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E93" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F93" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G93" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H93" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I93" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J93" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K93" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L93" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M93" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="N93" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="O93" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="P93" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q93" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="R93" s="22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="94" spans="2:18">
+      <c r="B94" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C94" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D94" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E94" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F94" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G94" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H94" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I94" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="J94" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K94" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="L94" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="M94" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="N94" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="O94" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="P94" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q94" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="R94" s="23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="95" spans="2:18">
+      <c r="B95" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C95" s="13"/>
+      <c r="D95" s="13"/>
+      <c r="E95" s="13"/>
+      <c r="F95" s="13"/>
+      <c r="G95" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H95" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I95" s="13"/>
+      <c r="J95" s="13"/>
+      <c r="K95" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="L95" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="M95" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="N95" s="13"/>
+      <c r="O95" s="13"/>
+      <c r="P95" s="13"/>
+      <c r="Q95" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="R95" s="24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="96" spans="2:18">
+      <c r="B96" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C96" s="13"/>
+      <c r="D96" s="13"/>
+      <c r="E96" s="13"/>
+      <c r="F96" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G96" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H96" s="13"/>
+      <c r="I96" s="13"/>
+      <c r="J96" s="13"/>
+      <c r="K96" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="L96" s="13"/>
+      <c r="M96" s="13"/>
+      <c r="N96" s="13"/>
+      <c r="O96" s="13"/>
+      <c r="P96" s="13"/>
+      <c r="Q96" s="13"/>
+      <c r="R96" s="26"/>
+    </row>
+    <row r="97" ht="15.15" spans="2:18">
+      <c r="B97" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C97" s="12"/>
+      <c r="D97" s="12"/>
+      <c r="E97" s="12"/>
+      <c r="F97" s="12"/>
+      <c r="G97" s="12"/>
+      <c r="H97" s="12"/>
+      <c r="I97" s="12"/>
+      <c r="J97" s="12"/>
+      <c r="K97" s="12"/>
+      <c r="L97" s="12"/>
+      <c r="M97" s="12"/>
+      <c r="N97" s="12"/>
+      <c r="O97" s="12"/>
+      <c r="P97" s="12"/>
+      <c r="Q97" s="12"/>
+      <c r="R97" s="27"/>
+    </row>
+    <row r="99" ht="15.15" spans="1:7">
+      <c r="A99" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B99" s="1"/>
+      <c r="C99" s="1"/>
+      <c r="D99" s="1"/>
+      <c r="E99" t="s">
+        <v>1</v>
+      </c>
+      <c r="F99" s="2" t="str">
+        <f>DEC2HEX(COUNTBLANK(C101:R104))</f>
+        <v>29</v>
+      </c>
+      <c r="G99" s="2" t="str">
+        <f>DEC2HEX(64)</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="100" spans="2:18">
+      <c r="B100" s="3"/>
+      <c r="C100" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D100" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E100" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F100" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G100" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H100" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I100" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J100" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K100" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L100" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M100" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="N100" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="O100" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="P100" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q100" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="R100" s="22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="101" spans="2:18">
+      <c r="B101" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C101" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D101" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E101" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F101" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G101" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H101" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I101" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="J101" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K101" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="L101" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="M101" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="N101" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="O101" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="P101" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q101" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="R101" s="23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="102" spans="2:18">
+      <c r="B102" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C102" s="13"/>
+      <c r="D102" s="13"/>
+      <c r="E102" s="13"/>
+      <c r="F102" s="13"/>
+      <c r="G102" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H102" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I102" s="13"/>
+      <c r="J102" s="13"/>
+      <c r="K102" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="L102" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="M102" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="N102" s="13"/>
+      <c r="O102" s="13"/>
+      <c r="P102" s="13"/>
+      <c r="Q102" s="13"/>
+      <c r="R102" s="26"/>
+    </row>
+    <row r="103" spans="2:18">
+      <c r="B103" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C103" s="13"/>
+      <c r="D103" s="13"/>
+      <c r="E103" s="13"/>
+      <c r="F103" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G103" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H103" s="13"/>
+      <c r="I103" s="13"/>
+      <c r="J103" s="13"/>
+      <c r="K103" s="13"/>
+      <c r="L103" s="13"/>
+      <c r="M103" s="13"/>
+      <c r="N103" s="13"/>
+      <c r="O103" s="13"/>
+      <c r="P103" s="13"/>
+      <c r="Q103" s="13"/>
+      <c r="R103" s="26"/>
+    </row>
+    <row r="104" ht="15.15" spans="2:18">
+      <c r="B104" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C104" s="12"/>
+      <c r="D104" s="12"/>
+      <c r="E104" s="12"/>
+      <c r="F104" s="12"/>
+      <c r="G104" s="12"/>
+      <c r="H104" s="12"/>
+      <c r="I104" s="12"/>
+      <c r="J104" s="12"/>
+      <c r="K104" s="12"/>
+      <c r="L104" s="12"/>
+      <c r="M104" s="12"/>
+      <c r="N104" s="12"/>
+      <c r="O104" s="12"/>
+      <c r="P104" s="12"/>
+      <c r="Q104" s="12"/>
+      <c r="R104" s="27"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="15">
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:J3"/>
-    <mergeCell ref="K3:N3"/>
-    <mergeCell ref="O3:R3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="A50:D50"/>
+    <mergeCell ref="A57:D57"/>
+    <mergeCell ref="A64:D64"/>
+    <mergeCell ref="A71:D71"/>
+    <mergeCell ref="A78:D78"/>
+    <mergeCell ref="A85:D85"/>
+    <mergeCell ref="A92:D92"/>
+    <mergeCell ref="A99:D99"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>